<commit_message>
added dropdown of fee in prediction
</commit_message>
<xml_diff>
--- a/20230901_account_balance_prediction.xlsx
+++ b/20230901_account_balance_prediction.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lab\DataAnalystCertificate\projects\ShodaClose\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C98B3FF6-0915-4F07-968C-C09823116E32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FD562F2-F090-4FF5-A74D-042AF685FC75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="24" yWindow="24" windowWidth="23016" windowHeight="12216" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -70,15 +70,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -86,15 +92,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -110,6 +132,1260 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>year</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2026</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2027</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2028</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2029</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2030</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2031</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2032</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2033</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7A2D-4BD3-A670-216A5651A582}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>balance</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>"$"#,##0.00_);[Red]\("$"#,##0.00\)</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)">
+                  <c:v>9955</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9825.8700000000008</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9573.678710000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9194.3651074300033</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8683.7341559751949</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8037.4523831223778</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7251.0433117654184</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6319.8827410536787</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5239.1938715084543</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4004.0422692682369</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2609.330664154093</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7A2D-4BD3-A670-216A5651A582}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>expense</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>3610</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3729.1299999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3852.1912899999993</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3979.3136025699991</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4110.6309514548084</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4246.2817728528171</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4386.4090713569594</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4531.1605707117387</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4680.6888695452253</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4835.1516022402175</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4994.7116051141438</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-7A2D-4BD3-A670-216A5651A582}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="844420831"/>
+        <c:axId val="846074127"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="3"/>
+                <c:order val="3"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$D$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>strata_fee</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent4"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$D$2:$D$12</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="11"/>
+                      <c:pt idx="0">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>50</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000003-7A2D-4BD3-A670-216A5651A582}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="4"/>
+                <c:order val="4"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$E$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>inflation_rate</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent5"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$E$2:$E$12</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>0.00%</c:formatCode>
+                      <c:ptCount val="11"/>
+                      <c:pt idx="0">
+                        <c:v>3.3000000000000002E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>3.3000000000000002E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>3.3000000000000002E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>3.3000000000000002E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>3.3000000000000002E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>3.3000000000000002E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>3.3000000000000002E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>3.3000000000000002E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>3.3000000000000002E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>3.3000000000000002E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>3.3000000000000002E-2</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000004-7A2D-4BD3-A670-216A5651A582}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="844420831"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="846074127"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="0"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="846074127"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="844420831"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>45720</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>163830</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>350520</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>163830</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3EBC6858-D114-7FCB-BD73-6FAAE3E28BA6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -378,7 +1654,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -387,7 +1663,7 @@
     <col min="5" max="5" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -404,7 +1680,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>2023</v>
       </c>
@@ -414,8 +1690,8 @@
       <c r="C2">
         <v>3610</v>
       </c>
-      <c r="D2">
-        <v>75</v>
+      <c r="D2" s="4">
+        <v>50</v>
       </c>
       <c r="E2" s="1">
         <v>3.3000000000000002E-2</v>
@@ -427,7 +1703,7 @@
       </c>
       <c r="B3" s="3">
         <f>B2+(D2*12*6)-C3</f>
-        <v>11625.87</v>
+        <v>9825.8700000000008</v>
       </c>
       <c r="C3">
         <f>C2*(1+E3)</f>
@@ -435,7 +1711,7 @@
       </c>
       <c r="D3">
         <f>$D$2</f>
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="E3" s="1">
         <v>3.3000000000000002E-2</v>
@@ -447,7 +1723,7 @@
       </c>
       <c r="B4" s="3">
         <f t="shared" ref="B4:B12" si="0">B3+(D3*12*6)-C4</f>
-        <v>13173.678710000004</v>
+        <v>9573.678710000002</v>
       </c>
       <c r="C4">
         <f t="shared" ref="C4:C12" si="1">C3*(1+E4)</f>
@@ -455,7 +1731,7 @@
       </c>
       <c r="D4">
         <f t="shared" ref="D4:D12" si="2">$D$2</f>
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="E4" s="1">
         <v>3.3000000000000002E-2</v>
@@ -467,7 +1743,7 @@
       </c>
       <c r="B5" s="3">
         <f t="shared" si="0"/>
-        <v>14594.365107430005</v>
+        <v>9194.3651074300033</v>
       </c>
       <c r="C5">
         <f t="shared" si="1"/>
@@ -475,7 +1751,7 @@
       </c>
       <c r="D5">
         <f t="shared" si="2"/>
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="E5" s="1">
         <v>3.3000000000000002E-2</v>
@@ -487,7 +1763,7 @@
       </c>
       <c r="B6" s="3">
         <f t="shared" si="0"/>
-        <v>15883.734155975199</v>
+        <v>8683.7341559751949</v>
       </c>
       <c r="C6">
         <f t="shared" si="1"/>
@@ -495,7 +1771,7 @@
       </c>
       <c r="D6">
         <f t="shared" si="2"/>
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="E6" s="1">
         <v>3.3000000000000002E-2</v>
@@ -507,7 +1783,7 @@
       </c>
       <c r="B7" s="3">
         <f t="shared" si="0"/>
-        <v>17037.452383122381</v>
+        <v>8037.4523831223778</v>
       </c>
       <c r="C7">
         <f t="shared" si="1"/>
@@ -515,7 +1791,7 @@
       </c>
       <c r="D7">
         <f t="shared" si="2"/>
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="E7" s="1">
         <v>3.3000000000000002E-2</v>
@@ -527,7 +1803,7 @@
       </c>
       <c r="B8" s="3">
         <f t="shared" si="0"/>
-        <v>18051.043311765421</v>
+        <v>7251.0433117654184</v>
       </c>
       <c r="C8">
         <f t="shared" si="1"/>
@@ -535,7 +1811,7 @@
       </c>
       <c r="D8">
         <f t="shared" si="2"/>
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="E8" s="1">
         <v>3.3000000000000002E-2</v>
@@ -547,7 +1823,7 @@
       </c>
       <c r="B9" s="3">
         <f t="shared" si="0"/>
-        <v>18919.882741053683</v>
+        <v>6319.8827410536787</v>
       </c>
       <c r="C9">
         <f t="shared" si="1"/>
@@ -555,7 +1831,7 @@
       </c>
       <c r="D9">
         <f t="shared" si="2"/>
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="E9" s="1">
         <v>3.3000000000000002E-2</v>
@@ -567,7 +1843,7 @@
       </c>
       <c r="B10" s="3">
         <f t="shared" si="0"/>
-        <v>19639.193871508458</v>
+        <v>5239.1938715084543</v>
       </c>
       <c r="C10">
         <f t="shared" si="1"/>
@@ -575,7 +1851,7 @@
       </c>
       <c r="D10">
         <f t="shared" si="2"/>
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="E10" s="1">
         <v>3.3000000000000002E-2</v>
@@ -587,7 +1863,7 @@
       </c>
       <c r="B11" s="3">
         <f t="shared" si="0"/>
-        <v>20204.04226926824</v>
+        <v>4004.0422692682369</v>
       </c>
       <c r="C11">
         <f t="shared" si="1"/>
@@ -595,7 +1871,7 @@
       </c>
       <c r="D11">
         <f t="shared" si="2"/>
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="E11" s="1">
         <v>3.3000000000000002E-2</v>
@@ -607,7 +1883,7 @@
       </c>
       <c r="B12" s="3">
         <f t="shared" si="0"/>
-        <v>20609.330664154098</v>
+        <v>2609.330664154093</v>
       </c>
       <c r="C12">
         <f t="shared" si="1"/>
@@ -615,7 +1891,7 @@
       </c>
       <c r="D12">
         <f t="shared" si="2"/>
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="E12" s="1">
         <v>3.3000000000000002E-2</v>
@@ -623,11 +1899,11 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" promptTitle="Edit this number" prompt="Edit the fee from 50-150 to see difference in yearly balance" sqref="D2" xr:uid="{F2209BBB-7A64-4CCF-9EDD-2B1BDDD0CEA6}">
-      <formula1>50</formula1>
-      <formula2>150</formula2>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="Edit this number" prompt="Edit the fee from 50-150 to see difference in yearly balance" sqref="D2" xr:uid="{F2209BBB-7A64-4CCF-9EDD-2B1BDDD0CEA6}">
+      <formula1>"50, 60, 70, 75, 80, 90, 100, 120, 150"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added expense estimate in prediction, optimized layout
</commit_message>
<xml_diff>
--- a/20230901_account_balance_prediction.xlsx
+++ b/20230901_account_balance_prediction.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lab\DataAnalystCertificate\projects\ShodaClose\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50EBFE06-FDE7-4858-A612-0B9E68189A39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{977BE56C-D8C5-4530-9D94-E3D9F561DF2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="24" yWindow="24" windowWidth="23016" windowHeight="12216" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>year</t>
   </si>
@@ -64,6 +64,42 @@
   <si>
     <t>* Change highlighted areas to see the trend of balance.</t>
   </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Account Balance Prediction</t>
+  </si>
+  <si>
+    <t>Annual Expenses Estimation</t>
+  </si>
+  <si>
+    <t>item</t>
+  </si>
+  <si>
+    <t>cost_per_year</t>
+  </si>
+  <si>
+    <t>water</t>
+  </si>
+  <si>
+    <t>insurance</t>
+  </si>
+  <si>
+    <t>grass_cutting</t>
+  </si>
+  <si>
+    <t>irrigation_test</t>
+  </si>
+  <si>
+    <t>snow_removal</t>
+  </si>
+  <si>
+    <t>electricity</t>
+  </si>
+  <si>
+    <t>Sum_of_expense</t>
+  </si>
 </sst>
 </file>
 
@@ -73,7 +109,7 @@
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0;[Red]\-&quot;$&quot;#,##0"/>
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,8 +117,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -101,8 +145,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -140,6 +190,21 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top/>
       <bottom style="medium">
@@ -153,6 +218,182 @@
         <color indexed="64"/>
       </right>
       <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -162,16 +403,32 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="6" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="6" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="6" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -224,16 +481,19 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-CA"/>
-              <a:t>Annual Changes in Account Balances</a:t>
+              <a:t>Annual Changes in Account Balances </a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-CA" baseline="0"/>
-              <a:t> </a:t>
-            </a:r>
-            <a:endParaRPr lang="en-CA"/>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.20063188976377955"/>
+          <c:y val="2.6809651474530832E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -274,7 +534,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$4</c:f>
+              <c:f>Sheet1!$B$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -295,9 +555,198 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-8.3333333333333332E-3"/>
+                  <c:y val="1.7873100983020553E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000E-1C72-4F76-A935-4D59D797DFAE}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-1C72-4F76-A935-4D59D797DFAE}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-1C72-4F76-A935-4D59D797DFAE}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000006-1C72-4F76-A935-4D59D797DFAE}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000007-1C72-4F76-A935-4D59D797DFAE}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000008-1C72-4F76-A935-4D59D797DFAE}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000A-1C72-4F76-A935-4D59D797DFAE}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000009-1C72-4F76-A935-4D59D797DFAE}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="8"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000C-1C72-4F76-A935-4D59D797DFAE}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="9"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000B-1C72-4F76-A935-4D59D797DFAE}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="10"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="-3.1277926720285967E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000D-1C72-4F76-A935-4D59D797DFAE}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$5:$A$15</c:f>
+              <c:f>Sheet1!$A$6:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -339,7 +788,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$5:$B$15</c:f>
+              <c:f>Sheet1!$B$6:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>"$"#,##0.00_);[Red]\("$"#,##0.00\)</c:formatCode>
                 <c:ptCount val="11"/>
@@ -347,34 +796,34 @@
                   <c:v>9955</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10752.470000000001</c:v>
+                  <c:v>10805.67</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11433.696510000002</c:v>
+                  <c:v>11553.732110000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11994.843494830002</c:v>
+                  <c:v>12195.800269630001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12431.948330159394</c:v>
+                  <c:v>12728.376678527791</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12740.917625054655</c:v>
+                  <c:v>13147.84810891921</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12917.522906681461</c:v>
+                  <c:v>13450.482096513544</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>12957.396162601952</c:v>
+                  <c:v>13632.423005698492</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>12856.025235967818</c:v>
+                  <c:v>13689.687964886545</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>12608.74906875476</c:v>
+                  <c:v>13618.162667727802</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>12210.75278802367</c:v>
+                  <c:v>13413.597035762825</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -391,7 +840,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$4</c:f>
+              <c:f>Sheet1!$C$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -414,7 +863,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$5:$A$15</c:f>
+              <c:f>Sheet1!$A$6:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -456,42 +905,42 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$5:$C$15</c:f>
+              <c:f>Sheet1!$C$6:$C$16</c:f>
               <c:numCache>
                 <c:formatCode>"$"#,##0_);[Red]\("$"#,##0\)</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>3410</c:v>
+                  <c:v>3010</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3522.5299999999997</c:v>
+                  <c:v>3109.33</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3638.7734899999996</c:v>
+                  <c:v>3211.9378899999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3758.8530151699993</c:v>
+                  <c:v>3317.9318403699995</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3882.8951646706091</c:v>
+                  <c:v>3427.4235911022092</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4011.0307051047389</c:v>
+                  <c:v>3540.5285696085821</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4143.3947183731952</c:v>
+                  <c:v>3657.3660124056651</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4280.12674407951</c:v>
+                  <c:v>3778.0590908150516</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4421.3709266341339</c:v>
+                  <c:v>3902.7350408119478</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4567.27616721306</c:v>
+                  <c:v>4031.5252971587415</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4717.9962807310903</c:v>
+                  <c:v>4164.5656319649797</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -508,7 +957,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$4</c:f>
+              <c:f>Sheet1!$D$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -531,7 +980,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$5:$A$15</c:f>
+              <c:f>Sheet1!$A$6:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -573,42 +1022,42 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$5:$D$15</c:f>
+              <c:f>Sheet1!$D$6:$D$16</c:f>
               <c:numCache>
                 <c:formatCode>"$"#,##0_);[Red]\("$"#,##0\)</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>4320</c:v>
+                  <c:v>3960</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4320</c:v>
+                  <c:v>3960</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4320</c:v>
+                  <c:v>3960</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4320</c:v>
+                  <c:v>3960</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4320</c:v>
+                  <c:v>3960</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4320</c:v>
+                  <c:v>3960</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4320</c:v>
+                  <c:v>3960</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4320</c:v>
+                  <c:v>3960</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4320</c:v>
+                  <c:v>3960</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4320</c:v>
+                  <c:v>3960</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4320</c:v>
+                  <c:v>3960</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1375,15 +1824,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>563880</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>87630</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>53340</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>83820</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:colOff>182880</xdr:colOff>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>87630</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1675,283 +2124,367 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="6">
-        <v>60</v>
+      <c r="B1" s="3">
+        <v>55</v>
       </c>
       <c r="C1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="7">
-        <v>3410</v>
+      <c r="B2" s="4">
+        <v>3010</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" t="s">
-        <v>3</v>
-      </c>
+    <row r="4" spans="1:5" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>2023</v>
-      </c>
-      <c r="B5" s="2">
-        <v>9955</v>
-      </c>
-      <c r="C5" s="8">
-        <f>$B$2</f>
-        <v>3410</v>
-      </c>
-      <c r="D5" s="2">
-        <f>$B$1*12*6</f>
-        <v>4320</v>
-      </c>
-      <c r="E5" s="1">
-        <v>3.3000000000000002E-2</v>
+      <c r="A5" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>2024</v>
-      </c>
-      <c r="B6" s="3">
-        <f>B5+D6-C6</f>
-        <v>10752.470000000001</v>
-      </c>
-      <c r="C6" s="8">
-        <f>C5*(1+E5)</f>
-        <v>3522.5299999999997</v>
-      </c>
-      <c r="D6" s="2">
-        <f t="shared" ref="D6:D15" si="0">$B$1*12*6</f>
-        <v>4320</v>
-      </c>
-      <c r="E6" s="1">
+      <c r="A6" s="7">
+        <v>2023</v>
+      </c>
+      <c r="B6" s="9">
+        <v>9955</v>
+      </c>
+      <c r="C6" s="9">
+        <f>$B$2</f>
+        <v>3010</v>
+      </c>
+      <c r="D6" s="9">
+        <f>$B$1*12*6</f>
+        <v>3960</v>
+      </c>
+      <c r="E6" s="5">
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>2025</v>
-      </c>
-      <c r="B7" s="3">
-        <f t="shared" ref="B7:B15" si="1">B6+D7-C7</f>
-        <v>11433.696510000002</v>
-      </c>
-      <c r="C7" s="8">
-        <f t="shared" ref="C7:C15" si="2">C6*(1+E6)</f>
-        <v>3638.7734899999996</v>
-      </c>
-      <c r="D7" s="2">
-        <f t="shared" si="0"/>
-        <v>4320</v>
-      </c>
-      <c r="E7" s="1">
+      <c r="A7" s="7">
+        <v>2024</v>
+      </c>
+      <c r="B7" s="10">
+        <f>B6+D7-C7</f>
+        <v>10805.67</v>
+      </c>
+      <c r="C7" s="12">
+        <f>C6*(1+E6)</f>
+        <v>3109.33</v>
+      </c>
+      <c r="D7" s="12">
+        <f t="shared" ref="D7:D16" si="0">$B$1*12*6</f>
+        <v>3960</v>
+      </c>
+      <c r="E7" s="5">
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>2026</v>
-      </c>
-      <c r="B8" s="3">
-        <f t="shared" si="1"/>
-        <v>11994.843494830002</v>
-      </c>
-      <c r="C8" s="8">
-        <f t="shared" si="2"/>
-        <v>3758.8530151699993</v>
-      </c>
-      <c r="D8" s="2">
+      <c r="A8" s="7">
+        <v>2025</v>
+      </c>
+      <c r="B8" s="10">
+        <f t="shared" ref="B8:B16" si="1">B7+D8-C8</f>
+        <v>11553.732110000001</v>
+      </c>
+      <c r="C8" s="12">
+        <f t="shared" ref="C8:C16" si="2">C7*(1+E7)</f>
+        <v>3211.9378899999997</v>
+      </c>
+      <c r="D8" s="12">
         <f t="shared" si="0"/>
-        <v>4320</v>
-      </c>
-      <c r="E8" s="1">
+        <v>3960</v>
+      </c>
+      <c r="E8" s="5">
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>2027</v>
-      </c>
-      <c r="B9" s="3">
+      <c r="A9" s="7">
+        <v>2026</v>
+      </c>
+      <c r="B9" s="10">
         <f t="shared" si="1"/>
-        <v>12431.948330159394</v>
-      </c>
-      <c r="C9" s="8">
+        <v>12195.800269630001</v>
+      </c>
+      <c r="C9" s="12">
         <f t="shared" si="2"/>
-        <v>3882.8951646706091</v>
-      </c>
-      <c r="D9" s="2">
+        <v>3317.9318403699995</v>
+      </c>
+      <c r="D9" s="12">
         <f t="shared" si="0"/>
-        <v>4320</v>
-      </c>
-      <c r="E9" s="1">
+        <v>3960</v>
+      </c>
+      <c r="E9" s="5">
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>2028</v>
-      </c>
-      <c r="B10" s="3">
+      <c r="A10" s="7">
+        <v>2027</v>
+      </c>
+      <c r="B10" s="10">
         <f t="shared" si="1"/>
-        <v>12740.917625054655</v>
-      </c>
-      <c r="C10" s="8">
+        <v>12728.376678527791</v>
+      </c>
+      <c r="C10" s="12">
         <f t="shared" si="2"/>
-        <v>4011.0307051047389</v>
-      </c>
-      <c r="D10" s="2">
+        <v>3427.4235911022092</v>
+      </c>
+      <c r="D10" s="12">
         <f t="shared" si="0"/>
-        <v>4320</v>
-      </c>
-      <c r="E10" s="1">
+        <v>3960</v>
+      </c>
+      <c r="E10" s="5">
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>2029</v>
-      </c>
-      <c r="B11" s="3">
+      <c r="A11" s="7">
+        <v>2028</v>
+      </c>
+      <c r="B11" s="10">
         <f t="shared" si="1"/>
-        <v>12917.522906681461</v>
-      </c>
-      <c r="C11" s="8">
+        <v>13147.84810891921</v>
+      </c>
+      <c r="C11" s="12">
         <f t="shared" si="2"/>
-        <v>4143.3947183731952</v>
-      </c>
-      <c r="D11" s="2">
+        <v>3540.5285696085821</v>
+      </c>
+      <c r="D11" s="12">
         <f t="shared" si="0"/>
-        <v>4320</v>
-      </c>
-      <c r="E11" s="1">
+        <v>3960</v>
+      </c>
+      <c r="E11" s="5">
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>2030</v>
-      </c>
-      <c r="B12" s="3">
+      <c r="A12" s="7">
+        <v>2029</v>
+      </c>
+      <c r="B12" s="10">
         <f t="shared" si="1"/>
-        <v>12957.396162601952</v>
-      </c>
-      <c r="C12" s="8">
+        <v>13450.482096513544</v>
+      </c>
+      <c r="C12" s="12">
         <f t="shared" si="2"/>
-        <v>4280.12674407951</v>
-      </c>
-      <c r="D12" s="2">
+        <v>3657.3660124056651</v>
+      </c>
+      <c r="D12" s="12">
         <f t="shared" si="0"/>
-        <v>4320</v>
-      </c>
-      <c r="E12" s="1">
+        <v>3960</v>
+      </c>
+      <c r="E12" s="5">
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>2031</v>
-      </c>
-      <c r="B13" s="3">
+      <c r="A13" s="7">
+        <v>2030</v>
+      </c>
+      <c r="B13" s="10">
         <f t="shared" si="1"/>
-        <v>12856.025235967818</v>
-      </c>
-      <c r="C13" s="8">
+        <v>13632.423005698492</v>
+      </c>
+      <c r="C13" s="12">
         <f t="shared" si="2"/>
-        <v>4421.3709266341339</v>
-      </c>
-      <c r="D13" s="2">
+        <v>3778.0590908150516</v>
+      </c>
+      <c r="D13" s="12">
         <f t="shared" si="0"/>
-        <v>4320</v>
-      </c>
-      <c r="E13" s="1">
+        <v>3960</v>
+      </c>
+      <c r="E13" s="5">
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>2032</v>
-      </c>
-      <c r="B14" s="3">
+      <c r="A14" s="7">
+        <v>2031</v>
+      </c>
+      <c r="B14" s="10">
         <f t="shared" si="1"/>
-        <v>12608.74906875476</v>
-      </c>
-      <c r="C14" s="8">
+        <v>13689.687964886545</v>
+      </c>
+      <c r="C14" s="12">
         <f t="shared" si="2"/>
-        <v>4567.27616721306</v>
-      </c>
-      <c r="D14" s="2">
+        <v>3902.7350408119478</v>
+      </c>
+      <c r="D14" s="12">
         <f t="shared" si="0"/>
-        <v>4320</v>
-      </c>
-      <c r="E14" s="1">
+        <v>3960</v>
+      </c>
+      <c r="E14" s="5">
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15">
+      <c r="A15" s="7">
+        <v>2032</v>
+      </c>
+      <c r="B15" s="10">
+        <f t="shared" si="1"/>
+        <v>13618.162667727802</v>
+      </c>
+      <c r="C15" s="12">
+        <f t="shared" si="2"/>
+        <v>4031.5252971587415</v>
+      </c>
+      <c r="D15" s="12">
+        <f t="shared" si="0"/>
+        <v>3960</v>
+      </c>
+      <c r="E15" s="5">
+        <v>3.3000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="8">
         <v>2033</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B16" s="11">
         <f t="shared" si="1"/>
-        <v>12210.75278802367</v>
-      </c>
-      <c r="C15" s="8">
+        <v>13413.597035762825</v>
+      </c>
+      <c r="C16" s="13">
         <f t="shared" si="2"/>
-        <v>4717.9962807310903</v>
-      </c>
-      <c r="D15" s="2">
+        <v>4164.5656319649797</v>
+      </c>
+      <c r="D16" s="13">
         <f t="shared" si="0"/>
-        <v>4320</v>
-      </c>
-      <c r="E15" s="1">
+        <v>3960</v>
+      </c>
+      <c r="E16" s="6">
         <v>3.3000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="22"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="18">
+        <v>250</v>
+      </c>
+      <c r="D20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" s="18">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" s="18">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" s="18">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" s="18">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" s="19">
+        <v>400</v>
+      </c>
+      <c r="D25" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="E25" s="21">
+        <v>3610</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="A18:B18"/>
+  </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="Click trangle to change number" prompt="number between 60-150" sqref="B1" xr:uid="{F2209BBB-7A64-4CCF-9EDD-2B1BDDD0CEA6}">
-      <formula1>"50, 60, 70, 75, 80, 90, 100, 120, 150"</formula1>
+      <formula1>"50, 55, 60, 65, 70, 75, 80, 90, 100, 120, 150"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Description" prompt="3610: include grass cutting and snow removal_x000a_3410: exclude grass cutting_x000a_3210: exclude snow removal_x000a_3010: exclude grass cutting and snow removal" sqref="B2" xr:uid="{1F41E19D-72B2-4CEC-8C8F-DB5BA9C7DB70}">
       <formula1>"3610, 3410, 3210, 3010"</formula1>

</xml_diff>

<commit_message>
created final version of prediction
</commit_message>
<xml_diff>
--- a/20230901_account_balance_prediction.xlsx
+++ b/20230901_account_balance_prediction.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lab\DataAnalystCertificate\projects\ShodaClose\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{977BE56C-D8C5-4530-9D94-E3D9F561DF2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8354C61-C965-49A5-BA45-37DB5F69A21A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="24" yWindow="24" windowWidth="23016" windowHeight="12216" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="chart&amp;data" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,8 +35,43 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Dongli</author>
+  </authors>
+  <commentList>
+    <comment ref="N5" authorId="0" shapeId="0" xr:uid="{0EDA7974-7EA4-41B7-B9D1-E2D1948AF9EB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Dongli:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+9955 # current balance
+- 290 # electricity+water</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>year</t>
   </si>
@@ -86,19 +121,48 @@
     <t>insurance</t>
   </si>
   <si>
-    <t>grass_cutting</t>
-  </si>
-  <si>
     <t>irrigation_test</t>
-  </si>
-  <si>
-    <t>snow_removal</t>
   </si>
   <si>
     <t>electricity</t>
   </si>
   <si>
     <t>Sum_of_expense</t>
+  </si>
+  <si>
+    <t>* Click data sheet to see details.</t>
+  </si>
+  <si>
+    <r>
+      <t>grass_cutting</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (opt)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">snow_removal </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(opt)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -109,8 +173,16 @@
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0;[Red]\-&quot;$&quot;#,##0"/>
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -125,8 +197,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -147,6 +232,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -403,7 +494,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -418,17 +509,20 @@
     <xf numFmtId="8" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -491,7 +585,7 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.20063188976377955"/>
-          <c:y val="2.6809651474530832E-2"/>
+          <c:y val="3.1326419563408231E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -534,7 +628,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$5</c:f>
+              <c:f>'chart&amp;data'!$N$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -702,7 +796,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -746,7 +840,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$6:$A$16</c:f>
+              <c:f>'chart&amp;data'!$M$5:$M$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -788,42 +882,42 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$6:$B$16</c:f>
+              <c:f>'chart&amp;data'!$N$5:$N$15</c:f>
               <c:numCache>
                 <c:formatCode>"$"#,##0.00_);[Red]\("$"#,##0.00\)</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)">
-                  <c:v>9955</c:v>
+                  <c:v>9665</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10805.67</c:v>
+                  <c:v>10462.470000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11553.732110000001</c:v>
+                  <c:v>11143.696510000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12195.800269630001</c:v>
+                  <c:v>11704.843494830002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12728.376678527791</c:v>
+                  <c:v>12141.948330159394</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13147.84810891921</c:v>
+                  <c:v>12450.917625054655</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>13450.482096513544</c:v>
+                  <c:v>12627.522906681461</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>13632.423005698492</c:v>
+                  <c:v>12667.396162601952</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>13689.687964886545</c:v>
+                  <c:v>12566.025235967818</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>13618.162667727802</c:v>
+                  <c:v>12318.74906875476</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>13413.597035762825</c:v>
+                  <c:v>11920.75278802367</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -840,7 +934,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$5</c:f>
+              <c:f>'chart&amp;data'!$O$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -863,7 +957,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$6:$A$16</c:f>
+              <c:f>'chart&amp;data'!$M$5:$M$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -905,42 +999,42 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$6:$C$16</c:f>
+              <c:f>'chart&amp;data'!$O$5:$O$15</c:f>
               <c:numCache>
                 <c:formatCode>"$"#,##0_);[Red]\("$"#,##0\)</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>3010</c:v>
+                  <c:v>3410</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3109.33</c:v>
+                  <c:v>3522.5299999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3211.9378899999997</c:v>
+                  <c:v>3638.7734899999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3317.9318403699995</c:v>
+                  <c:v>3758.8530151699993</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3427.4235911022092</c:v>
+                  <c:v>3882.8951646706091</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3540.5285696085821</c:v>
+                  <c:v>4011.0307051047389</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3657.3660124056651</c:v>
+                  <c:v>4143.3947183731952</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3778.0590908150516</c:v>
+                  <c:v>4280.12674407951</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3902.7350408119478</c:v>
+                  <c:v>4421.3709266341339</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4031.5252971587415</c:v>
+                  <c:v>4567.27616721306</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4164.5656319649797</c:v>
+                  <c:v>4717.9962807310903</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -957,7 +1051,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$5</c:f>
+              <c:f>'chart&amp;data'!$P$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -980,7 +1074,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$6:$A$16</c:f>
+              <c:f>'chart&amp;data'!$M$5:$M$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1022,42 +1116,42 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$6:$D$16</c:f>
+              <c:f>'chart&amp;data'!$P$5:$P$15</c:f>
               <c:numCache>
                 <c:formatCode>"$"#,##0_);[Red]\("$"#,##0\)</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>3960</c:v>
+                  <c:v>4320</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3960</c:v>
+                  <c:v>4320</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3960</c:v>
+                  <c:v>4320</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3960</c:v>
+                  <c:v>4320</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3960</c:v>
+                  <c:v>4320</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3960</c:v>
+                  <c:v>4320</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3960</c:v>
+                  <c:v>4320</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3960</c:v>
+                  <c:v>4320</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3960</c:v>
+                  <c:v>4320</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3960</c:v>
+                  <c:v>4320</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3960</c:v>
+                  <c:v>4320</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1824,16 +1918,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>53340</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>11430</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>182880</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>87630</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>198120</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2123,374 +2217,381 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2:Q24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="2" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="2:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="3">
-        <v>55</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="C3" s="3">
+        <v>60</v>
+      </c>
+      <c r="D3" t="s">
         <v>8</v>
       </c>
+      <c r="M3" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="21"/>
+      <c r="Q3" s="21"/>
     </row>
-    <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+    <row r="4" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="4">
-        <v>3010</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="C4" s="4">
+        <v>3410</v>
+      </c>
+      <c r="D4" t="s">
         <v>6</v>
       </c>
+      <c r="M4" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="N4" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="O4" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="P4" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q4" s="17" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="M5" s="7">
+        <v>2023</v>
+      </c>
+      <c r="N5" s="9">
+        <v>9665</v>
+      </c>
+      <c r="O5" s="9">
+        <f>'chart&amp;data'!$C$4</f>
+        <v>3410</v>
+      </c>
+      <c r="P5" s="9">
+        <f>'chart&amp;data'!$C$3*12*6</f>
+        <v>4320</v>
+      </c>
+      <c r="Q5" s="5">
+        <v>3.3000000000000002E-2</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="17" t="s">
-        <v>3</v>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="M6" s="7">
+        <v>2024</v>
+      </c>
+      <c r="N6" s="10">
+        <f>N5+P6-O6</f>
+        <v>10462.470000000001</v>
+      </c>
+      <c r="O6" s="12">
+        <f>O5*(1+Q5)</f>
+        <v>3522.5299999999997</v>
+      </c>
+      <c r="P6" s="12">
+        <f>'chart&amp;data'!$C$3*12*6</f>
+        <v>4320</v>
+      </c>
+      <c r="Q6" s="5">
+        <v>3.3000000000000002E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="7">
-        <v>2023</v>
-      </c>
-      <c r="B6" s="9">
-        <v>9955</v>
-      </c>
-      <c r="C6" s="9">
-        <f>$B$2</f>
-        <v>3010</v>
-      </c>
-      <c r="D6" s="9">
-        <f>$B$1*12*6</f>
-        <v>3960</v>
-      </c>
-      <c r="E6" s="5">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="M7" s="7">
+        <v>2025</v>
+      </c>
+      <c r="N7" s="10">
+        <f>N6+P7-O7</f>
+        <v>11143.696510000002</v>
+      </c>
+      <c r="O7" s="12">
+        <f>O6*(1+Q6)</f>
+        <v>3638.7734899999996</v>
+      </c>
+      <c r="P7" s="12">
+        <f>'chart&amp;data'!$C$3*12*6</f>
+        <v>4320</v>
+      </c>
+      <c r="Q7" s="5">
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="7">
-        <v>2024</v>
-      </c>
-      <c r="B7" s="10">
-        <f>B6+D7-C7</f>
-        <v>10805.67</v>
-      </c>
-      <c r="C7" s="12">
-        <f>C6*(1+E6)</f>
-        <v>3109.33</v>
-      </c>
-      <c r="D7" s="12">
-        <f t="shared" ref="D7:D16" si="0">$B$1*12*6</f>
-        <v>3960</v>
-      </c>
-      <c r="E7" s="5">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="M8" s="7">
+        <v>2026</v>
+      </c>
+      <c r="N8" s="10">
+        <f>N7+P8-O8</f>
+        <v>11704.843494830002</v>
+      </c>
+      <c r="O8" s="12">
+        <f>O7*(1+Q7)</f>
+        <v>3758.8530151699993</v>
+      </c>
+      <c r="P8" s="12">
+        <f>'chart&amp;data'!$C$3*12*6</f>
+        <v>4320</v>
+      </c>
+      <c r="Q8" s="5">
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="7">
-        <v>2025</v>
-      </c>
-      <c r="B8" s="10">
-        <f t="shared" ref="B8:B16" si="1">B7+D8-C8</f>
-        <v>11553.732110000001</v>
-      </c>
-      <c r="C8" s="12">
-        <f t="shared" ref="C8:C16" si="2">C7*(1+E7)</f>
-        <v>3211.9378899999997</v>
-      </c>
-      <c r="D8" s="12">
-        <f t="shared" si="0"/>
-        <v>3960</v>
-      </c>
-      <c r="E8" s="5">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="M9" s="7">
+        <v>2027</v>
+      </c>
+      <c r="N9" s="10">
+        <f>N8+P9-O9</f>
+        <v>12141.948330159394</v>
+      </c>
+      <c r="O9" s="12">
+        <f>O8*(1+Q8)</f>
+        <v>3882.8951646706091</v>
+      </c>
+      <c r="P9" s="12">
+        <f>'chart&amp;data'!$C$3*12*6</f>
+        <v>4320</v>
+      </c>
+      <c r="Q9" s="5">
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="7">
-        <v>2026</v>
-      </c>
-      <c r="B9" s="10">
-        <f t="shared" si="1"/>
-        <v>12195.800269630001</v>
-      </c>
-      <c r="C9" s="12">
-        <f t="shared" si="2"/>
-        <v>3317.9318403699995</v>
-      </c>
-      <c r="D9" s="12">
-        <f t="shared" si="0"/>
-        <v>3960</v>
-      </c>
-      <c r="E9" s="5">
+    <row r="10" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="M10" s="7">
+        <v>2028</v>
+      </c>
+      <c r="N10" s="10">
+        <f>N9+P10-O10</f>
+        <v>12450.917625054655</v>
+      </c>
+      <c r="O10" s="12">
+        <f>O9*(1+Q9)</f>
+        <v>4011.0307051047389</v>
+      </c>
+      <c r="P10" s="12">
+        <f>'chart&amp;data'!$C$3*12*6</f>
+        <v>4320</v>
+      </c>
+      <c r="Q10" s="5">
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="7">
-        <v>2027</v>
-      </c>
-      <c r="B10" s="10">
-        <f t="shared" si="1"/>
-        <v>12728.376678527791</v>
-      </c>
-      <c r="C10" s="12">
-        <f t="shared" si="2"/>
-        <v>3427.4235911022092</v>
-      </c>
-      <c r="D10" s="12">
-        <f t="shared" si="0"/>
-        <v>3960</v>
-      </c>
-      <c r="E10" s="5">
+    <row r="11" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="M11" s="7">
+        <v>2029</v>
+      </c>
+      <c r="N11" s="10">
+        <f>N10+P11-O11</f>
+        <v>12627.522906681461</v>
+      </c>
+      <c r="O11" s="12">
+        <f>O10*(1+Q10)</f>
+        <v>4143.3947183731952</v>
+      </c>
+      <c r="P11" s="12">
+        <f>'chart&amp;data'!$C$3*12*6</f>
+        <v>4320</v>
+      </c>
+      <c r="Q11" s="5">
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="7">
-        <v>2028</v>
-      </c>
-      <c r="B11" s="10">
-        <f t="shared" si="1"/>
-        <v>13147.84810891921</v>
-      </c>
-      <c r="C11" s="12">
-        <f t="shared" si="2"/>
-        <v>3540.5285696085821</v>
-      </c>
-      <c r="D11" s="12">
-        <f t="shared" si="0"/>
-        <v>3960</v>
-      </c>
-      <c r="E11" s="5">
+    <row r="12" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="M12" s="7">
+        <v>2030</v>
+      </c>
+      <c r="N12" s="10">
+        <f>N11+P12-O12</f>
+        <v>12667.396162601952</v>
+      </c>
+      <c r="O12" s="12">
+        <f>O11*(1+Q11)</f>
+        <v>4280.12674407951</v>
+      </c>
+      <c r="P12" s="12">
+        <f>'chart&amp;data'!$C$3*12*6</f>
+        <v>4320</v>
+      </c>
+      <c r="Q12" s="5">
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="7">
-        <v>2029</v>
-      </c>
-      <c r="B12" s="10">
-        <f t="shared" si="1"/>
-        <v>13450.482096513544</v>
-      </c>
-      <c r="C12" s="12">
-        <f t="shared" si="2"/>
-        <v>3657.3660124056651</v>
-      </c>
-      <c r="D12" s="12">
-        <f t="shared" si="0"/>
-        <v>3960</v>
-      </c>
-      <c r="E12" s="5">
+    <row r="13" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="M13" s="7">
+        <v>2031</v>
+      </c>
+      <c r="N13" s="10">
+        <f>N12+P13-O13</f>
+        <v>12566.025235967818</v>
+      </c>
+      <c r="O13" s="12">
+        <f>O12*(1+Q12)</f>
+        <v>4421.3709266341339</v>
+      </c>
+      <c r="P13" s="12">
+        <f>'chart&amp;data'!$C$3*12*6</f>
+        <v>4320</v>
+      </c>
+      <c r="Q13" s="5">
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="7">
-        <v>2030</v>
-      </c>
-      <c r="B13" s="10">
-        <f t="shared" si="1"/>
-        <v>13632.423005698492</v>
-      </c>
-      <c r="C13" s="12">
-        <f t="shared" si="2"/>
-        <v>3778.0590908150516</v>
-      </c>
-      <c r="D13" s="12">
-        <f t="shared" si="0"/>
-        <v>3960</v>
-      </c>
-      <c r="E13" s="5">
+    <row r="14" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="M14" s="7">
+        <v>2032</v>
+      </c>
+      <c r="N14" s="10">
+        <f>N13+P14-O14</f>
+        <v>12318.74906875476</v>
+      </c>
+      <c r="O14" s="12">
+        <f>O13*(1+Q13)</f>
+        <v>4567.27616721306</v>
+      </c>
+      <c r="P14" s="12">
+        <f>'chart&amp;data'!$C$3*12*6</f>
+        <v>4320</v>
+      </c>
+      <c r="Q14" s="5">
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="7">
-        <v>2031</v>
-      </c>
-      <c r="B14" s="10">
-        <f t="shared" si="1"/>
-        <v>13689.687964886545</v>
-      </c>
-      <c r="C14" s="12">
-        <f t="shared" si="2"/>
-        <v>3902.7350408119478</v>
-      </c>
-      <c r="D14" s="12">
-        <f t="shared" si="0"/>
-        <v>3960</v>
-      </c>
-      <c r="E14" s="5">
+    <row r="15" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="M15" s="8">
+        <v>2033</v>
+      </c>
+      <c r="N15" s="11">
+        <f>N14+P15-O15</f>
+        <v>11920.75278802367</v>
+      </c>
+      <c r="O15" s="13">
+        <f>O14*(1+Q14)</f>
+        <v>4717.9962807310903</v>
+      </c>
+      <c r="P15" s="13">
+        <f>'chart&amp;data'!$C$3*12*6</f>
+        <v>4320</v>
+      </c>
+      <c r="Q15" s="6">
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="7">
-        <v>2032</v>
-      </c>
-      <c r="B15" s="10">
-        <f t="shared" si="1"/>
-        <v>13618.162667727802</v>
-      </c>
-      <c r="C15" s="12">
-        <f t="shared" si="2"/>
-        <v>4031.5252971587415</v>
-      </c>
-      <c r="D15" s="12">
-        <f t="shared" si="0"/>
-        <v>3960</v>
-      </c>
-      <c r="E15" s="5">
-        <v>3.3000000000000002E-2</v>
-      </c>
+    <row r="17" spans="13:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="M17" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="N17" s="21"/>
     </row>
-    <row r="16" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="8">
-        <v>2033</v>
-      </c>
-      <c r="B16" s="11">
-        <f t="shared" si="1"/>
-        <v>13413.597035762825</v>
-      </c>
-      <c r="C16" s="13">
-        <f t="shared" si="2"/>
-        <v>4164.5656319649797</v>
-      </c>
-      <c r="D16" s="13">
-        <f t="shared" si="0"/>
-        <v>3960</v>
-      </c>
-      <c r="E16" s="6">
-        <v>3.3000000000000002E-2</v>
+    <row r="18" spans="13:17" x14ac:dyDescent="0.3">
+      <c r="M18" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="N18" s="17" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="B18" s="22"/>
+    <row r="19" spans="13:17" x14ac:dyDescent="0.3">
+      <c r="M19" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="N19" s="18">
+        <v>250</v>
+      </c>
+      <c r="P19" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B19" s="17" t="s">
-        <v>13</v>
+    <row r="20" spans="13:17" x14ac:dyDescent="0.3">
+      <c r="M20" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="N20" s="18">
+        <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20" s="18">
-        <v>250</v>
-      </c>
-      <c r="D20" t="s">
-        <v>9</v>
+    <row r="21" spans="13:17" x14ac:dyDescent="0.3">
+      <c r="M21" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="N21" s="18">
+        <v>2500</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B21" s="18">
-        <v>60</v>
+    <row r="22" spans="13:17" x14ac:dyDescent="0.3">
+      <c r="M22" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="N22" s="23">
+        <v>200</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B22" s="18">
-        <v>2500</v>
+    <row r="23" spans="13:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="M23" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="N23" s="18">
+        <v>200</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B23" s="18">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B24" s="18">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="8" t="s">
+    <row r="24" spans="13:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="M24" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="N24" s="25">
+        <v>400</v>
+      </c>
+      <c r="P24" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B25" s="19">
-        <v>400</v>
-      </c>
-      <c r="D25" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="E25" s="21">
+      <c r="Q24" s="20">
         <v>3610</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="M3:Q3"/>
+    <mergeCell ref="M17:N17"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="Click trangle to change number" prompt="number between 60-150" sqref="B1" xr:uid="{F2209BBB-7A64-4CCF-9EDD-2B1BDDD0CEA6}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{F2209BBB-7A64-4CCF-9EDD-2B1BDDD0CEA6}">
       <formula1>"50, 55, 60, 65, 70, 75, 80, 90, 100, 120, 150"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Description" prompt="3610: include grass cutting and snow removal_x000a_3410: exclude grass cutting_x000a_3210: exclude snow removal_x000a_3010: exclude grass cutting and snow removal" sqref="B2" xr:uid="{1F41E19D-72B2-4CEC-8C8F-DB5BA9C7DB70}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Description" prompt="3610: +SnowRemoval, +GrassCut_x000a_3410: +SnowRemoval_x000a_3210: +GrassCut_x000a_3010: None" sqref="C4" xr:uid="{1F41E19D-72B2-4CEC-8C8F-DB5BA9C7DB70}">
       <formula1>"3610, 3410, 3210, 3010"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added $ in dropdown list for compatibility in GoogleSheet
</commit_message>
<xml_diff>
--- a/20230901_account_balance_prediction.xlsx
+++ b/20230901_account_balance_prediction.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lab\DataAnalystCertificate\projects\ShodaClose\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8354C61-C965-49A5-BA45-37DB5F69A21A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47BE09F1-15BC-42D7-BE73-6D92708622FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="24" yWindow="24" windowWidth="23016" windowHeight="12216" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -514,15 +514,15 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2221,7 +2221,7 @@
   <dimension ref="B2:Q24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2250,13 +2250,13 @@
       <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="M3" s="21" t="s">
+      <c r="M3" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="N3" s="21"/>
-      <c r="O3" s="21"/>
-      <c r="P3" s="21"/>
-      <c r="Q3" s="21"/>
+      <c r="N3" s="25"/>
+      <c r="O3" s="25"/>
+      <c r="P3" s="25"/>
+      <c r="Q3" s="25"/>
     </row>
     <row r="4" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
@@ -2311,11 +2311,11 @@
         <v>2024</v>
       </c>
       <c r="N6" s="10">
-        <f>N5+P6-O6</f>
+        <f t="shared" ref="N6:N15" si="0">N5+P6-O6</f>
         <v>10462.470000000001</v>
       </c>
       <c r="O6" s="12">
-        <f>O5*(1+Q5)</f>
+        <f t="shared" ref="O6:O15" si="1">O5*(1+Q5)</f>
         <v>3522.5299999999997</v>
       </c>
       <c r="P6" s="12">
@@ -2331,11 +2331,11 @@
         <v>2025</v>
       </c>
       <c r="N7" s="10">
-        <f>N6+P7-O7</f>
+        <f t="shared" si="0"/>
         <v>11143.696510000002</v>
       </c>
       <c r="O7" s="12">
-        <f>O6*(1+Q6)</f>
+        <f t="shared" si="1"/>
         <v>3638.7734899999996</v>
       </c>
       <c r="P7" s="12">
@@ -2351,11 +2351,11 @@
         <v>2026</v>
       </c>
       <c r="N8" s="10">
-        <f>N7+P8-O8</f>
+        <f t="shared" si="0"/>
         <v>11704.843494830002</v>
       </c>
       <c r="O8" s="12">
-        <f>O7*(1+Q7)</f>
+        <f t="shared" si="1"/>
         <v>3758.8530151699993</v>
       </c>
       <c r="P8" s="12">
@@ -2371,11 +2371,11 @@
         <v>2027</v>
       </c>
       <c r="N9" s="10">
-        <f>N8+P9-O9</f>
+        <f t="shared" si="0"/>
         <v>12141.948330159394</v>
       </c>
       <c r="O9" s="12">
-        <f>O8*(1+Q8)</f>
+        <f t="shared" si="1"/>
         <v>3882.8951646706091</v>
       </c>
       <c r="P9" s="12">
@@ -2391,11 +2391,11 @@
         <v>2028</v>
       </c>
       <c r="N10" s="10">
-        <f>N9+P10-O10</f>
+        <f t="shared" si="0"/>
         <v>12450.917625054655</v>
       </c>
       <c r="O10" s="12">
-        <f>O9*(1+Q9)</f>
+        <f t="shared" si="1"/>
         <v>4011.0307051047389</v>
       </c>
       <c r="P10" s="12">
@@ -2411,11 +2411,11 @@
         <v>2029</v>
       </c>
       <c r="N11" s="10">
-        <f>N10+P11-O11</f>
+        <f t="shared" si="0"/>
         <v>12627.522906681461</v>
       </c>
       <c r="O11" s="12">
-        <f>O10*(1+Q10)</f>
+        <f t="shared" si="1"/>
         <v>4143.3947183731952</v>
       </c>
       <c r="P11" s="12">
@@ -2431,11 +2431,11 @@
         <v>2030</v>
       </c>
       <c r="N12" s="10">
-        <f>N11+P12-O12</f>
+        <f t="shared" si="0"/>
         <v>12667.396162601952</v>
       </c>
       <c r="O12" s="12">
-        <f>O11*(1+Q11)</f>
+        <f t="shared" si="1"/>
         <v>4280.12674407951</v>
       </c>
       <c r="P12" s="12">
@@ -2451,11 +2451,11 @@
         <v>2031</v>
       </c>
       <c r="N13" s="10">
-        <f>N12+P13-O13</f>
+        <f t="shared" si="0"/>
         <v>12566.025235967818</v>
       </c>
       <c r="O13" s="12">
-        <f>O12*(1+Q12)</f>
+        <f t="shared" si="1"/>
         <v>4421.3709266341339</v>
       </c>
       <c r="P13" s="12">
@@ -2471,11 +2471,11 @@
         <v>2032</v>
       </c>
       <c r="N14" s="10">
-        <f>N13+P14-O14</f>
+        <f t="shared" si="0"/>
         <v>12318.74906875476</v>
       </c>
       <c r="O14" s="12">
-        <f>O13*(1+Q13)</f>
+        <f t="shared" si="1"/>
         <v>4567.27616721306</v>
       </c>
       <c r="P14" s="12">
@@ -2491,11 +2491,11 @@
         <v>2033</v>
       </c>
       <c r="N15" s="11">
-        <f>N14+P15-O15</f>
+        <f t="shared" si="0"/>
         <v>11920.75278802367</v>
       </c>
       <c r="O15" s="13">
-        <f>O14*(1+Q14)</f>
+        <f t="shared" si="1"/>
         <v>4717.9962807310903</v>
       </c>
       <c r="P15" s="13">
@@ -2507,10 +2507,10 @@
       </c>
     </row>
     <row r="17" spans="13:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="M17" s="21" t="s">
+      <c r="M17" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="N17" s="21"/>
+      <c r="N17" s="25"/>
     </row>
     <row r="18" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M18" s="14" t="s">
@@ -2548,10 +2548,10 @@
       </c>
     </row>
     <row r="22" spans="13:17" x14ac:dyDescent="0.3">
-      <c r="M22" s="22" t="s">
+      <c r="M22" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="N22" s="23">
+      <c r="N22" s="22">
         <v>200</v>
       </c>
     </row>
@@ -2564,10 +2564,10 @@
       </c>
     </row>
     <row r="24" spans="13:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="M24" s="24" t="s">
+      <c r="M24" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="N24" s="25">
+      <c r="N24" s="24">
         <v>400</v>
       </c>
       <c r="P24" s="19" t="s">
@@ -2584,14 +2584,15 @@
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{F2209BBB-7A64-4CCF-9EDD-2B1BDDD0CEA6}">
-      <formula1>"50, 55, 60, 65, 70, 75, 80, 90, 100, 120, 150"</formula1>
+      <formula1>"$50, $55, $60, $65, $70, $75, $80, $90, $100, $120, $150"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Description" prompt="3610: +SnowRemoval, +GrassCut_x000a_3410: +SnowRemoval_x000a_3210: +GrassCut_x000a_3010: None" sqref="C4" xr:uid="{1F41E19D-72B2-4CEC-8C8F-DB5BA9C7DB70}">
-      <formula1>"3610, 3410, 3210, 3010"</formula1>
+      <formula1>"$3610, $3410, $3210, $3010"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>